<commit_message>
Add Bootstrap and Quarto assets, update thesis files
Added Bootstrap and Quarto library assets for improved styling and interactivity. Updated codebook, thesis, SAP, and index files, as well as generated HTML and JSON outputs to reflect latest content and formatting.
</commit_message>
<xml_diff>
--- a/docs/Codebook_Cigarette.xlsx
+++ b/docs/Codebook_Cigarette.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Graduate Courses\PHPH 7990\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\myechow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394FDBCD-8615-45C2-9164-A220FCD5784F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D289B9F6-6AD4-44AD-9D74-66870981D8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{576F2D76-5E76-4B83-A195-30915DF4AE14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
   <si>
     <t>att1</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>Which grade are you in?</t>
-  </si>
-  <si>
-    <t>plh1</t>
   </si>
   <si>
     <t>V7666</t>
@@ -539,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -667,6 +664,29 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1004,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAE1A3D-1F19-459C-869A-2138E75B477E}">
   <dimension ref="A1:E813"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1020,16 +1040,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="38"/>
+      <c r="A2" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="47"/>
       <c r="C2" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="38"/>
       <c r="E2" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1043,7 +1063,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>1</v>
@@ -1054,55 +1074,55 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="39"/>
+      <c r="A6" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="45"/>
       <c r="C6" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="39"/>
       <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>7</v>
@@ -1113,28 +1133,28 @@
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="39"/>
+      <c r="A9" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="45"/>
       <c r="C9" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="39"/>
       <c r="E9" s="32"/>
@@ -1161,7 +1181,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>12</v>
@@ -1170,113 +1190,113 @@
         <v>11</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="34"/>
+      <c r="A12" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="48"/>
       <c r="C12" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="34"/>
+      <c r="A14" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="48"/>
       <c r="C14" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="16" t="s">
+      <c r="B16" s="50"/>
+      <c r="C16" s="40" t="s">
         <v>37</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="40" t="s">
-        <v>38</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="34"/>
+      <c r="A18" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="48"/>
       <c r="C18" s="42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="43"/>
       <c r="E18" s="14"/>
     </row>
     <row r="19" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>14</v>
@@ -1286,31 +1306,31 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="36"/>
+      <c r="A20" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="52"/>
       <c r="C20" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="36"/>
       <c r="E20" s="11"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="B21" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="E21" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1324,7 +1344,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>16</v>
@@ -1335,7 +1355,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>18</v>
@@ -1358,7 +1378,7 @@
         <v>21</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>22</v>
@@ -6875,9 +6895,7 @@
       <c r="E813" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A20:B20"/>
+  <mergeCells count="8">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C9:D9"/>
@@ -6886,12 +6904,6 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>